<commit_message>
23/12 Update design and task
</commit_message>
<xml_diff>
--- a/doc/checklist/PQ01_checklist.xlsx
+++ b/doc/checklist/PQ01_checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="23520" windowHeight="16590"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="23520" windowHeight="16596"/>
   </bookViews>
   <sheets>
     <sheet name="To Do List" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="Grid" localSheetId="0">ToDoList[[#All],[Description]:[Assigned to]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'To Do List'!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm\.dd\.yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -545,7 +545,397 @@
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="8" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="180">
+  <dxfs count="232">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <u val="none"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
@@ -1899,14 +2289,14 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="To Do List" defaultPivotStyle="PivotStyleLight18">
     <tableStyle name="Address Book" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" dxfId="179"/>
-      <tableStyleElement type="headerRow" dxfId="178"/>
-      <tableStyleElement type="firstRowStripe" dxfId="177"/>
-      <tableStyleElement type="secondRowStripe" dxfId="176"/>
+      <tableStyleElement type="wholeTable" dxfId="231"/>
+      <tableStyleElement type="headerRow" dxfId="230"/>
+      <tableStyleElement type="firstRowStripe" dxfId="229"/>
+      <tableStyleElement type="secondRowStripe" dxfId="228"/>
     </tableStyle>
     <tableStyle name="To Do List" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="175"/>
-      <tableStyleElement type="headerRow" dxfId="174"/>
+      <tableStyleElement type="wholeTable" dxfId="227"/>
+      <tableStyleElement type="headerRow" dxfId="226"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1947,7 +2337,7 @@
         <xdr:cNvPr id="4" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2024,7 +2414,7 @@
         <xdr:cNvPr id="16" name="Data Entry Tip" descr="Enter a number greater than 1 in Done column when  task is complete">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1954A24D-DF3A-439E-AB30-634556E8A9EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2193,7 +2583,7 @@
         <xdr:cNvPr id="17" name="Picture 16" descr="Decorative element&#10;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF377864-4FEB-4775-90CF-2A6C6DFF8FD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2240,18 +2630,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ToDoList" displayName="ToDoList" ref="B6:H17" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ToDoList" displayName="ToDoList" ref="B6:H17" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="B6:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Done" dataDxfId="8"/>
-    <tableColumn id="2" name="Description" dataDxfId="7"/>
-    <tableColumn id="3" name="Due Date" dataDxfId="6"/>
-    <tableColumn id="4" name="Priority" dataDxfId="5"/>
-    <tableColumn id="5" name="Assigned to" dataDxfId="4"/>
-    <tableColumn id="8" name="Date Modify" dataDxfId="3">
+    <tableColumn id="1" name="Done" dataDxfId="60"/>
+    <tableColumn id="2" name="Description" dataDxfId="59"/>
+    <tableColumn id="3" name="Due Date" dataDxfId="58"/>
+    <tableColumn id="4" name="Priority" dataDxfId="57"/>
+    <tableColumn id="5" name="Assigned to" dataDxfId="56"/>
+    <tableColumn id="8" name="Date Modify" dataDxfId="55">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Update " dataDxfId="2"/>
+    <tableColumn id="6" name="Update " dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="Address Book" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2263,7 +2653,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ColorKeys" displayName="ColorKeys" ref="B3:B7" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ColorKeys" displayName="ColorKeys" ref="B3:B7" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52">
   <tableColumns count="1">
     <tableColumn id="1" name="Assigned To"/>
   </tableColumns>
@@ -2510,24 +2900,24 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="17.21875" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1796875" style="4" hidden="1" customWidth="1"/>
     <col min="11" max="15" width="0" style="4" hidden="1" customWidth="1"/>
     <col min="16" max="18" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.77734375" style="2" hidden="1"/>
+    <col min="19" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="66" customHeight="1">
@@ -2583,7 +2973,7 @@
       </c>
       <c r="C3" s="23">
         <f ca="1">COUNTIFS(ToDoList[Due Date],TODAY(),ToDoList[Done],"&lt;&gt;1")</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -2669,7 +3059,9 @@
       <c r="A7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
       <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
@@ -2807,8 +3199,8 @@
         <v>20</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" ref="G11:G14" ca="1" si="1">TODAY()</f>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="H11" s="28" t="s">
         <v>20</v>
@@ -2829,8 +3221,8 @@
         <v>29</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" ref="D12:D17" ca="1" si="2">TODAY()</f>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>5</v>
@@ -2839,8 +3231,8 @@
         <v>21</v>
       </c>
       <c r="G12" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>21</v>
@@ -2861,8 +3253,8 @@
         <v>30</v>
       </c>
       <c r="D13" s="6">
-        <f t="shared" ca="1" si="2"/>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>6</v>
@@ -2871,8 +3263,8 @@
         <v>20</v>
       </c>
       <c r="G13" s="6">
-        <f t="shared" ca="1" si="1"/>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="H13" s="28" t="s">
         <v>20</v>
@@ -2890,7 +3282,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="D12:D17" ca="1" si="1">TODAY()</f>
         <v>43457</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -2900,7 +3292,7 @@
         <v>22</v>
       </c>
       <c r="G14" s="6">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="G11:G14" ca="1" si="2">TODAY()</f>
         <v>43457</v>
       </c>
       <c r="H14" s="28" t="s">
@@ -2921,8 +3313,8 @@
         <v>32</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" ca="1" si="2"/>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>5</v>
@@ -2931,8 +3323,8 @@
         <v>21</v>
       </c>
       <c r="G15" s="6">
-        <f ca="1">TODAY()</f>
-        <v>43457</v>
+        <f ca="1">TODAY()-1</f>
+        <v>43456</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -2942,7 +3334,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>43457</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -2956,12 +3348,14 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:15" ht="30" customHeight="1">
-      <c r="B17" s="29"/>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
       <c r="C17" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="6">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>43457</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2986,589 +3380,631 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <conditionalFormatting sqref="C11:C12 C7:C8">
-    <cfRule type="expression" dxfId="173" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="225" priority="244" stopIfTrue="1">
       <formula>D7=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:E8 C11:E12 E9:E10">
-    <cfRule type="expression" dxfId="172" priority="218" stopIfTrue="1">
+  <conditionalFormatting sqref="C7:E8 E9:E10 C11:E12">
+    <cfRule type="expression" dxfId="224" priority="242" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="219">
+    <cfRule type="expression" dxfId="223" priority="243">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="221">
+    <cfRule type="expression" dxfId="222" priority="245">
       <formula>AND(B7&lt;&gt;1,D7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="222">
+    <cfRule type="expression" dxfId="221" priority="246">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:F14">
-    <cfRule type="expression" dxfId="168" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="266" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="243">
+    <cfRule type="expression" dxfId="219" priority="267">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="244">
+    <cfRule type="expression" dxfId="218" priority="268">
       <formula>AND(E7&lt;&gt;1,I7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="245">
+    <cfRule type="expression" dxfId="217" priority="269">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="164" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="270" stopIfTrue="1">
       <formula>$B8=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="247">
+    <cfRule type="expression" dxfId="215" priority="271">
       <formula>$D8=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="248">
+    <cfRule type="expression" dxfId="214" priority="272">
       <formula>AND(F8&lt;&gt;1,J8=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="249">
+    <cfRule type="expression" dxfId="213" priority="273">
       <formula>AND($B8&lt;&gt;1,$D8&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G14">
-    <cfRule type="expression" dxfId="160" priority="209" stopIfTrue="1">
+  <conditionalFormatting sqref="G7:G10 G14">
+    <cfRule type="expression" dxfId="212" priority="233" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="210">
+    <cfRule type="expression" dxfId="211" priority="234">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="211">
+    <cfRule type="expression" dxfId="210" priority="235">
       <formula>AND(F7&lt;&gt;1,H7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="212">
+    <cfRule type="expression" dxfId="209" priority="236">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="expression" dxfId="156" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="229" stopIfTrue="1">
       <formula>$B7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="206">
+    <cfRule type="expression" dxfId="207" priority="230">
       <formula>$D7=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="207">
+    <cfRule type="expression" dxfId="206" priority="231">
       <formula>AND(G7&lt;&gt;1,K7=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="208">
+    <cfRule type="expression" dxfId="205" priority="232">
       <formula>AND($B7&lt;&gt;1,$D7&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="152" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="226" stopIfTrue="1">
       <formula>D9=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="151" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="224" stopIfTrue="1">
       <formula>$B9=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="201">
+    <cfRule type="expression" dxfId="202" priority="225">
       <formula>$D9=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="203">
+    <cfRule type="expression" dxfId="201" priority="227">
       <formula>AND(B9&lt;&gt;1,D9=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="204">
+    <cfRule type="expression" dxfId="200" priority="228">
       <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="147" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="221" stopIfTrue="1">
       <formula>D10=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="146" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="219" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="196">
+    <cfRule type="expression" dxfId="197" priority="220">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="198">
+    <cfRule type="expression" dxfId="196" priority="222">
       <formula>AND(B10&lt;&gt;1,D10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="199">
+    <cfRule type="expression" dxfId="195" priority="223">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="142" priority="191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="215" stopIfTrue="1">
       <formula>$B11=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="192">
+    <cfRule type="expression" dxfId="193" priority="216">
       <formula>$D11=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="193">
+    <cfRule type="expression" dxfId="192" priority="217">
       <formula>AND(G11&lt;&gt;1,K11=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="194">
+    <cfRule type="expression" dxfId="191" priority="218">
       <formula>AND($B11&lt;&gt;1,$D11&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="138" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="211" stopIfTrue="1">
       <formula>$B12=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="188">
+    <cfRule type="expression" dxfId="189" priority="212">
       <formula>$D12=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="189">
+    <cfRule type="expression" dxfId="188" priority="213">
       <formula>AND(G12&lt;&gt;1,K12=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="190">
+    <cfRule type="expression" dxfId="187" priority="214">
       <formula>AND($B12&lt;&gt;1,$D12&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="134" priority="183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="207" stopIfTrue="1">
       <formula>$B10=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="184">
+    <cfRule type="expression" dxfId="185" priority="208">
       <formula>$D10=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="185">
+    <cfRule type="expression" dxfId="184" priority="209">
       <formula>AND(G10&lt;&gt;1,K10=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="186">
+    <cfRule type="expression" dxfId="183" priority="210">
       <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="130" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="204" stopIfTrue="1">
       <formula>D13=""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="129" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="202" stopIfTrue="1">
       <formula>$B13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="179">
+    <cfRule type="expression" dxfId="180" priority="203">
       <formula>$D13=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="181">
+    <cfRule type="expression" dxfId="179" priority="205">
       <formula>AND(B13&lt;&gt;1,D13=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="182">
+    <cfRule type="expression" dxfId="178" priority="206">
       <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="expression" dxfId="173" priority="194" stopIfTrue="1">
+      <formula>$B13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="172" priority="195">
+      <formula>$D13=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="171" priority="196">
+      <formula>AND(D13&lt;&gt;1,F13=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="170" priority="197">
+      <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
+    <cfRule type="expression" dxfId="169" priority="190" stopIfTrue="1">
+      <formula>$B13=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="168" priority="191">
+      <formula>$D13=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="167" priority="192">
+      <formula>AND(G13&lt;&gt;1,K13=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="166" priority="193">
+      <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="expression" dxfId="165" priority="186" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="164" priority="187">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="163" priority="188">
+      <formula>AND(G9&lt;&gt;1,K9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="162" priority="189">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="expression" dxfId="161" priority="182" stopIfTrue="1">
+      <formula>$B14=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="160" priority="183">
+      <formula>$D14=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="159" priority="184">
+      <formula>AND(D14&lt;&gt;1,F14=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="158" priority="185">
+      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14">
+    <cfRule type="expression" dxfId="157" priority="178" stopIfTrue="1">
+      <formula>$B14=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="156" priority="179">
+      <formula>$D14=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="155" priority="180">
+      <formula>AND(C14&lt;&gt;1,E14=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="154" priority="181">
+      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14">
+    <cfRule type="expression" dxfId="153" priority="174" stopIfTrue="1">
+      <formula>$B14=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="152" priority="175">
+      <formula>$D14=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="151" priority="176">
+      <formula>AND(G14&lt;&gt;1,K14=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="150" priority="177">
+      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="149" priority="171" stopIfTrue="1">
+      <formula>D14=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="148" priority="169" stopIfTrue="1">
+      <formula>$B14=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="147" priority="170">
+      <formula>$D14=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="146" priority="172">
+      <formula>AND(B14&lt;&gt;1,D14=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="145" priority="173">
+      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="expression" dxfId="144" priority="144" stopIfTrue="1">
+      <formula>$B15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="143" priority="145">
+      <formula>$D15=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="146">
+      <formula>AND(D15&lt;&gt;1,F15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="141" priority="147">
+      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="expression" dxfId="140" priority="149" stopIfTrue="1">
+      <formula>$B15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="139" priority="150">
+      <formula>$D15=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="151">
+      <formula>AND(E15&lt;&gt;1,I15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="137" priority="152">
+      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="136" priority="137" stopIfTrue="1">
+      <formula>D15=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="135" priority="135" stopIfTrue="1">
+      <formula>$B15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="136">
+      <formula>$D15=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="133" priority="138">
+      <formula>AND(B15&lt;&gt;1,D15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="139">
+      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="expression" dxfId="131" priority="131" stopIfTrue="1">
+      <formula>$B15=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="130" priority="132">
+      <formula>$D15=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="129" priority="133">
+      <formula>AND(G15&lt;&gt;1,K15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="128" priority="134">
+      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="127" priority="122" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="126" priority="123">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="125" priority="124">
+      <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="124" priority="125">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="123" priority="127" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="122" priority="128">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="121" priority="129">
+      <formula>AND(E16&lt;&gt;1,I16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="120" priority="130">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="119" priority="115" stopIfTrue="1">
+      <formula>D16=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="118" priority="113" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="114">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="116">
+      <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="117">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="expression" dxfId="114" priority="109" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="113" priority="110">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="112" priority="111">
+      <formula>AND(G16&lt;&gt;1,K16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="111" priority="112">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="expression" dxfId="106" priority="101" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="105" priority="102">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="104" priority="103">
+      <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="103" priority="104">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="expression" dxfId="98" priority="93" stopIfTrue="1">
+      <formula>$B16=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="97" priority="94">
+      <formula>$D16=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="95">
+      <formula>AND(F16&lt;&gt;1,H16=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="95" priority="96">
+      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="expression" dxfId="94" priority="89" stopIfTrue="1">
+      <formula>$B9=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="93" priority="90">
+      <formula>$D9=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="92" priority="91">
+      <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="91" priority="92">
+      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="90" priority="85" stopIfTrue="1">
+      <formula>$B10=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="89" priority="86">
+      <formula>$D10=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="88" priority="87">
+      <formula>AND(C10&lt;&gt;1,E10=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="87" priority="88">
+      <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="expression" dxfId="86" priority="55" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="85" priority="56">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="84" priority="57">
+      <formula>AND(E17&lt;&gt;1,I17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="83" priority="58">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="expression" dxfId="82" priority="50" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="81" priority="51">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="80" priority="52">
+      <formula>AND(F17&lt;&gt;1,H17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="79" priority="53">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="78" priority="47" stopIfTrue="1">
+      <formula>D17=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="expression" dxfId="77" priority="45" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="46">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="75" priority="48">
+      <formula>AND(B17&lt;&gt;1,D17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="74" priority="49">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17">
+    <cfRule type="expression" dxfId="73" priority="41" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="72" priority="42">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="71" priority="43">
+      <formula>AND(C17&lt;&gt;1,E17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="70" priority="44">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="expression" dxfId="69" priority="29" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="68" priority="30">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="67" priority="31">
+      <formula>AND(G17&lt;&gt;1,K17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="66" priority="32">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="expression" dxfId="65" priority="25" stopIfTrue="1">
+      <formula>$B17=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="64" priority="26">
+      <formula>$D17=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="27">
+      <formula>AND(D17&lt;&gt;1,F17=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="28">
+      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="125" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="21" stopIfTrue="1">
       <formula>$B13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="175">
+    <cfRule type="expression" dxfId="50" priority="22">
       <formula>$D13=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="176">
+    <cfRule type="expression" dxfId="49" priority="23">
       <formula>AND(C13&lt;&gt;1,E13=TODAY())</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="177">
+    <cfRule type="expression" dxfId="48" priority="24">
       <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="121" priority="170" stopIfTrue="1">
+  <conditionalFormatting sqref="G11">
+    <cfRule type="expression" dxfId="39" priority="17" stopIfTrue="1">
+      <formula>$B11=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="18">
+      <formula>$D11=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="19">
+      <formula>AND(F11&lt;&gt;1,H11=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="20">
+      <formula>AND($B11&lt;&gt;1,$D11&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="expression" dxfId="31" priority="13" stopIfTrue="1">
+      <formula>$B12=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="14">
+      <formula>$D12=TODAY()</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="15">
+      <formula>AND(F12&lt;&gt;1,H12=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="16">
+      <formula>AND($B12&lt;&gt;1,$D12&lt;TODAY())</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="expression" dxfId="23" priority="9" stopIfTrue="1">
       <formula>$B13=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="171">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>$D13=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="172">
-      <formula>AND(D13&lt;&gt;1,F13=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="118" priority="173">
+    <cfRule type="expression" dxfId="21" priority="11">
+      <formula>AND(F13&lt;&gt;1,H13=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="12">
       <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="117" priority="166" stopIfTrue="1">
-      <formula>$B13=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="167">
-      <formula>$D13=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="115" priority="168">
-      <formula>AND(G13&lt;&gt;1,K13=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="114" priority="169">
-      <formula>AND($B13&lt;&gt;1,$D13&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="113" priority="162" stopIfTrue="1">
-      <formula>$B9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="112" priority="163">
-      <formula>$D9=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="111" priority="164">
-      <formula>AND(G9&lt;&gt;1,K9=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="110" priority="165">
-      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="109" priority="158" stopIfTrue="1">
-      <formula>$B14=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="108" priority="159">
-      <formula>$D14=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="107" priority="160">
-      <formula>AND(D14&lt;&gt;1,F14=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="106" priority="161">
-      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="105" priority="154" stopIfTrue="1">
-      <formula>$B14=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="104" priority="155">
-      <formula>$D14=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="103" priority="156">
-      <formula>AND(C14&lt;&gt;1,E14=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="102" priority="157">
-      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14">
-    <cfRule type="expression" dxfId="101" priority="150" stopIfTrue="1">
-      <formula>$B14=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="100" priority="151">
-      <formula>$D14=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="99" priority="152">
-      <formula>AND(G14&lt;&gt;1,K14=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="98" priority="153">
-      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="97" priority="147" stopIfTrue="1">
-      <formula>D14=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="96" priority="145" stopIfTrue="1">
-      <formula>$B14=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="95" priority="146">
-      <formula>$D14=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="94" priority="148">
-      <formula>AND(B14&lt;&gt;1,D14=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="93" priority="149">
-      <formula>AND($B14&lt;&gt;1,$D14&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="92" priority="120" stopIfTrue="1">
+  <conditionalFormatting sqref="G15">
+    <cfRule type="expression" dxfId="15" priority="5" stopIfTrue="1">
       <formula>$B15=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="121">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>$D15=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="122">
-      <formula>AND(D15&lt;&gt;1,F15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="89" priority="123">
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>AND(F15&lt;&gt;1,H15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="88" priority="125" stopIfTrue="1">
+  <conditionalFormatting sqref="D15">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>$B15=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="126">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$D15=TODAY()</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="127">
-      <formula>AND(E15&lt;&gt;1,I15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="128">
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>AND(C15&lt;&gt;1,E15=TODAY())</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="84" priority="113" stopIfTrue="1">
-      <formula>D15=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="83" priority="111" stopIfTrue="1">
-      <formula>$B15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="112">
-      <formula>$D15=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="114">
-      <formula>AND(B15&lt;&gt;1,D15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="80" priority="115">
-      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="79" priority="107" stopIfTrue="1">
-      <formula>$B15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="78" priority="108">
-      <formula>$D15=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="77" priority="109">
-      <formula>AND(G15&lt;&gt;1,K15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="110">
-      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="75" priority="98" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="74" priority="99">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="73" priority="100">
-      <formula>AND(D16&lt;&gt;1,F16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="72" priority="101">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="71" priority="103" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="104">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="105">
-      <formula>AND(E16&lt;&gt;1,I16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="106">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="67" priority="91" stopIfTrue="1">
-      <formula>D16=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="66" priority="89" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="90">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="92">
-      <formula>AND(B16&lt;&gt;1,D16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="93">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="62" priority="85" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="86">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="87">
-      <formula>AND(G16&lt;&gt;1,K16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="88">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="58" priority="81" stopIfTrue="1">
-      <formula>$B15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="82">
-      <formula>$D15=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="83">
-      <formula>AND(C15&lt;&gt;1,E15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="84">
-      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="54" priority="77" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="78">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="79">
-      <formula>AND(C16&lt;&gt;1,E16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="80">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
-    <cfRule type="expression" dxfId="50" priority="73" stopIfTrue="1">
-      <formula>$B15=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="74">
-      <formula>$D15=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="48" priority="75">
-      <formula>AND(F15&lt;&gt;1,H15=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="76">
-      <formula>AND($B15&lt;&gt;1,$D15&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="expression" dxfId="46" priority="69" stopIfTrue="1">
-      <formula>$B16=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="70">
-      <formula>$D16=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="71">
-      <formula>AND(F16&lt;&gt;1,H16=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="72">
-      <formula>AND($B16&lt;&gt;1,$D16&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="42" priority="65" stopIfTrue="1">
-      <formula>$B9=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="66">
-      <formula>$D9=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="67">
-      <formula>AND(C9&lt;&gt;1,E9=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="68">
-      <formula>AND($B9&lt;&gt;1,$D9&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="38" priority="61" stopIfTrue="1">
-      <formula>$B10=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="62">
-      <formula>$D10=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="63">
-      <formula>AND(C10&lt;&gt;1,E10=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="64">
-      <formula>AND($B10&lt;&gt;1,$D10&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
-    <cfRule type="expression" dxfId="34" priority="31" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="32">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="33">
-      <formula>AND(E17&lt;&gt;1,I17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="34">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
-    <cfRule type="expression" dxfId="30" priority="26" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>AND(F17&lt;&gt;1,H17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="26" priority="23" stopIfTrue="1">
-      <formula>D17=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="25" priority="21" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="22">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="24">
-      <formula>AND(B17&lt;&gt;1,D17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="25">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="21" priority="17" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="18">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="19">
-      <formula>AND(C17&lt;&gt;1,E17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="6">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="7">
-      <formula>AND(G17&lt;&gt;1,K17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
-      <formula>$B17=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
-      <formula>$D17=TODAY()</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>AND(D17&lt;&gt;1,F17=TODAY())</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4">
-      <formula>AND($B17&lt;&gt;1,$D17&lt;TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="17">
@@ -3610,7 +4046,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="223" id="{BA82746F-AAF3-49E9-901A-F6FDFCCA8AAC}">
+          <x14:cfRule type="iconSet" priority="247" id="{BA82746F-AAF3-49E9-901A-F6FDFCCA8AAC}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3629,7 +4065,7 @@
           <xm:sqref>B7:B14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="124" id="{72DBEF15-DA85-40DA-A573-1193ECB69020}">
+          <x14:cfRule type="iconSet" priority="148" id="{72DBEF15-DA85-40DA-A573-1193ECB69020}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3648,7 +4084,7 @@
           <xm:sqref>B15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="102" id="{0D2FC9E8-E461-4F78-9C5A-6A697C458083}">
+          <x14:cfRule type="iconSet" priority="126" id="{0D2FC9E8-E461-4F78-9C5A-6A697C458083}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3667,7 +4103,7 @@
           <xm:sqref>B16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="30" id="{A94F79BD-CBE4-48BA-BEF8-9630C5323DC2}">
+          <x14:cfRule type="iconSet" priority="54" id="{A94F79BD-CBE4-48BA-BEF8-9630C5323DC2}">
             <x14:iconSet iconSet="3Symbols2" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3705,13 +4141,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.21875" style="2" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="8.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="15" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.77734375" style="2" hidden="1"/>
+    <col min="16" max="16384" width="10.81640625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="66" customHeight="1">
@@ -3799,6 +4235,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4006,25 +4460,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7118F064-9046-4DCB-A010-2D274D0FB549}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4042,22 +4496,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{920DC3BD-3C4B-4C78-91FF-63EB10F70D2C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CCC4C8-6A95-4999-B963-115A022CA31F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>